<commit_message>
Add toolchain identification to checklist
Signed-off-by: MikeOpenHWGroup <mike@openhwgroup.org>
</commit_message>
<xml_diff>
--- a/program/milestones/templates/OpenHWGroup_TRL3_for_COREV_RTL_IP_Template.xlsx
+++ b/program/milestones/templates/OpenHWGroup_TRL3_for_COREV_RTL_IP_Template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="1" state="visible" r:id="rId2"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="144">
   <si>
     <t xml:space="preserve">Copyright 2022 by the OpenHW Group</t>
   </si>
@@ -451,6 +451,21 @@
   </si>
   <si>
     <t xml:space="preserve">Coverage Results</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Toolchain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What software toolchain (cross-compiler, linker) was used for this project?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Provide location of toolchain:
+1. Publically accessible URL (e.g. a GitHub repository).
+2. Reference to GNU or LLVM toolchain version.
+3. Commerical platform (e.g. Embecosm).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cannot be waived unless a toolchain was not used.</t>
   </si>
 </sst>
 </file>
@@ -730,11 +745,11 @@
   </sheetPr>
   <dimension ref="B2:B22"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="84"/>
@@ -845,7 +860,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.42"/>
@@ -1055,7 +1070,7 @@
       <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.42"/>
@@ -1437,7 +1452,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.42"/>
@@ -1698,11 +1713,11 @@
   </sheetPr>
   <dimension ref="B2:F3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.42"/>
@@ -1729,8 +1744,20 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="0" t="s">
+        <v>140</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>142</v>
+      </c>
       <c r="E3" s="18"/>
+      <c r="F3" s="0" t="s">
+        <v>143</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Respond to DBees feedback
Signed-off-by: MikeOpenHWGroup <mike@openhwgroup.org>
</commit_message>
<xml_diff>
--- a/program/milestones/templates/OpenHWGroup_TRL3_for_COREV_RTL_IP_Template.xlsx
+++ b/program/milestones/templates/OpenHWGroup_TRL3_for_COREV_RTL_IP_Template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="1" state="visible" r:id="rId2"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="145">
   <si>
     <t xml:space="preserve">Copyright 2022 by the OpenHW Group</t>
   </si>
@@ -38,6 +38,12 @@
     <t xml:space="preserve">This document is the Checklist for TRL-3 criteria for OpenHW Group RTL IP.</t>
   </si>
   <si>
+    <t xml:space="preserve">Open Source Audits</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All Source code and contributions are reviewed under the Eclipse Development Process unless otherwise stated.</t>
+  </si>
+  <si>
     <t xml:space="preserve">RTL IP</t>
   </si>
   <si>
@@ -50,7 +56,7 @@
     <t xml:space="preserve">Technical Readiness Level 3. CORE-V IP that means the TRL-3 criteria is stable, validated against a specific software toolchain and implements a proof-of-concept.  It is not expected to be “production ready”.</t>
   </si>
   <si>
-    <t xml:space="preserve">Deliverables: OpenHW provides the following at RTL Freeze:</t>
+    <t xml:space="preserve">Deliverables: OpenHW provides the following at TRL-3:</t>
   </si>
   <si>
     <t xml:space="preserve">- A complete User Manual including implementation guidelines</t>
@@ -95,7 +101,7 @@
     <t xml:space="preserve">User Manual</t>
   </si>
   <si>
-    <t xml:space="preserve">Tagged version of source available in core-v-docs</t>
+    <t xml:space="preserve">Tagged version of source available in specified CORE-V repository.</t>
   </si>
   <si>
     <t xml:space="preserve">Formally released static version attributed to core-v-docs tag</t>
@@ -159,9 +165,6 @@
   </si>
   <si>
     <t xml:space="preserve">The version at this release is clearly identified in GitHub and in the RTL freeze review document.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">arjan.bink@silabs.com</t>
   </si>
   <si>
     <t xml:space="preserve">Coding rules</t>
@@ -589,7 +592,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -603,6 +606,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -743,13 +750,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B2:B22"/>
+  <dimension ref="B2:B25"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="84"/>
@@ -778,15 +785,18 @@
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="3"/>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="2" t="s">
+    <row r="8" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="3" t="s">
         <v>5</v>
       </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="3"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="2" t="s">
@@ -803,39 +813,49 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="0" t="s">
+    <row r="15" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="0" t="s">
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B17" s="2" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="0" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B20" s="0" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="2" t="s">
+    <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B21" s="0" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="3" t="s">
+    <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B22" s="0" t="s">
         <v>15</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B24" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B25" s="3" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -860,186 +880,186 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="38.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="51.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="55.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="22.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="51.13"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2" s="4" t="s">
+      <c r="B2" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="C2" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="D2" s="5" t="s">
         <v>20</v>
       </c>
+      <c r="E2" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B3" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D3" s="7" t="s">
+      <c r="B3" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E3" s="8"/>
-      <c r="F3" s="7"/>
+      <c r="C3" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" s="9"/>
+      <c r="F3" s="8"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="5"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="5"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="5"/>
-      <c r="C6" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B7" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="D7" s="7" t="s">
+      <c r="B7" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
+      <c r="C7" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="5"/>
-      <c r="C8" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="D8" s="7" t="s">
+      <c r="B8" s="6"/>
+      <c r="C8" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B9" s="6"/>
+      <c r="C9" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="5"/>
-      <c r="C9" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="5"/>
-      <c r="C10" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="5"/>
-      <c r="C11" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="5"/>
-      <c r="C12" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="5"/>
-      <c r="C13" s="6" t="s">
+      <c r="B13" s="6"/>
+      <c r="C13" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="D13" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="D13" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="5"/>
-      <c r="C14" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="5"/>
-      <c r="C15" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="5"/>
-      <c r="C16" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="D16" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1070,7 +1090,7 @@
       <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.42"/>
@@ -1081,346 +1101,344 @@
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2" s="4" t="s">
+      <c r="B2" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="C2" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="D2" s="5" t="s">
         <v>20</v>
       </c>
+      <c r="E2" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="D3" s="9" t="s">
+      <c r="B3" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="C3" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="F3" s="9"/>
+      <c r="D3" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="E3" s="11"/>
+      <c r="F3" s="10"/>
     </row>
     <row r="4" customFormat="false" ht="124.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B4" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="C4" s="9" t="s">
+      <c r="B4" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="C4" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
+      <c r="D4" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="5"/>
-      <c r="C5" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="D5" s="9" t="s">
+      <c r="B5" s="6"/>
+      <c r="C5" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
+      <c r="D5" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
     </row>
     <row r="6" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="5"/>
-      <c r="C6" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="D6" s="9" t="s">
+      <c r="B6" s="6"/>
+      <c r="C6" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9" t="s">
+      <c r="D6" s="10" t="s">
         <v>53</v>
       </c>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="5"/>
-      <c r="C7" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="D7" s="12" t="s">
+      <c r="B7" s="6"/>
+      <c r="C7" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12" t="s">
+      <c r="D7" s="13" t="s">
         <v>56</v>
       </c>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="5"/>
-      <c r="C8" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="D8" s="12" t="s">
+      <c r="B8" s="6"/>
+      <c r="C8" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
+      <c r="D8" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
     </row>
     <row r="9" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="5"/>
-      <c r="C9" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="D9" s="12" t="s">
+      <c r="B9" s="6"/>
+      <c r="C9" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12" t="s">
+      <c r="D9" s="13" t="s">
         <v>61</v>
       </c>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="5"/>
-      <c r="C10" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="D10" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="E10" s="12"/>
-      <c r="F10" s="13"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="E10" s="13"/>
+      <c r="F10" s="14"/>
     </row>
     <row r="11" customFormat="false" ht="46.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B11" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="C11" s="9" t="s">
+      <c r="B11" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="D11" s="12" t="s">
+      <c r="C11" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="E11" s="12"/>
-      <c r="F11" s="9"/>
+      <c r="D11" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="E11" s="13"/>
+      <c r="F11" s="10"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="5"/>
-      <c r="C12" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="D12" s="9" t="s">
+      <c r="B12" s="6"/>
+      <c r="C12" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
+      <c r="D12" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10"/>
     </row>
     <row r="13" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="5"/>
-      <c r="C13" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="D13" s="9" t="s">
+      <c r="B13" s="6"/>
+      <c r="C13" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="E13" s="9"/>
-      <c r="F13" s="9" t="s">
+      <c r="D13" s="10" t="s">
         <v>70</v>
       </c>
+      <c r="E13" s="10"/>
+      <c r="F13" s="10" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="5"/>
-      <c r="C14" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="D14" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="E14" s="9"/>
-      <c r="F14" s="9"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="E14" s="10"/>
+      <c r="F14" s="10"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="5"/>
-      <c r="C15" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="D15" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="E15" s="9"/>
-      <c r="F15" s="9"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="E15" s="10"/>
+      <c r="F15" s="10"/>
     </row>
     <row r="16" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="5"/>
-      <c r="C16" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="D16" s="9" t="s">
+      <c r="B16" s="6"/>
+      <c r="C16" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="E16" s="9"/>
-      <c r="F16" s="9" t="s">
+      <c r="D16" s="10" t="s">
         <v>75</v>
       </c>
+      <c r="E16" s="10"/>
+      <c r="F16" s="10" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="5"/>
-      <c r="C17" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="D17" s="9" t="s">
+      <c r="B17" s="6"/>
+      <c r="C17" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="E17" s="9"/>
-      <c r="F17" s="9" t="s">
+      <c r="D17" s="10" t="s">
         <v>78</v>
       </c>
+      <c r="E17" s="10"/>
+      <c r="F17" s="10" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="5"/>
-      <c r="C18" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="D18" s="9" t="s">
+      <c r="B18" s="6"/>
+      <c r="C18" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="E18" s="9"/>
-      <c r="F18" s="9"/>
+      <c r="D18" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="E18" s="10"/>
+      <c r="F18" s="10"/>
     </row>
     <row r="19" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="5"/>
-      <c r="C19" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="D19" s="12" t="s">
+      <c r="B19" s="6"/>
+      <c r="C19" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="E19" s="12"/>
-      <c r="F19" s="9"/>
+      <c r="D19" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="E19" s="13"/>
+      <c r="F19" s="10"/>
     </row>
     <row r="20" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="5"/>
-      <c r="C20" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="D20" s="9" t="s">
+      <c r="B20" s="6"/>
+      <c r="C20" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="E20" s="9"/>
-      <c r="F20" s="9" t="s">
+      <c r="D20" s="10" t="s">
         <v>85</v>
       </c>
+      <c r="E20" s="10"/>
+      <c r="F20" s="10" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="5"/>
-      <c r="C21" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="D21" s="9" t="s">
+      <c r="B21" s="6"/>
+      <c r="C21" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="E21" s="9"/>
-      <c r="F21" s="9"/>
+      <c r="D21" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="E21" s="10"/>
+      <c r="F21" s="10"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="5"/>
-      <c r="C22" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="D22" s="9" t="s">
+      <c r="B22" s="6"/>
+      <c r="C22" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="E22" s="9"/>
-      <c r="F22" s="9"/>
+      <c r="D22" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="E22" s="10"/>
+      <c r="F22" s="10"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="5"/>
-      <c r="C23" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="D23" s="9" t="s">
+      <c r="B23" s="6"/>
+      <c r="C23" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="E23" s="9"/>
-      <c r="F23" s="9" t="s">
+      <c r="D23" s="10" t="s">
         <v>92</v>
       </c>
+      <c r="E23" s="10"/>
+      <c r="F23" s="10" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="C24" s="9" t="s">
+      <c r="B24" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="D24" s="9" t="s">
+      <c r="C24" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="E24" s="10"/>
-      <c r="F24" s="9"/>
+      <c r="D24" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="E24" s="11"/>
+      <c r="F24" s="10"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B25" s="14" t="s">
-        <v>96</v>
-      </c>
-      <c r="C25" s="9" t="s">
+      <c r="B25" s="15" t="s">
         <v>97</v>
       </c>
-      <c r="D25" s="12" t="s">
+      <c r="C25" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="E25" s="12"/>
-      <c r="F25" s="9"/>
+      <c r="D25" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="E25" s="13"/>
+      <c r="F25" s="10"/>
     </row>
     <row r="26" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="14"/>
-      <c r="C26" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="D26" s="9" t="s">
+      <c r="B26" s="15"/>
+      <c r="C26" s="10" t="s">
         <v>100</v>
       </c>
-      <c r="E26" s="9"/>
-      <c r="F26" s="9"/>
+      <c r="D26" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="E26" s="10"/>
+      <c r="F26" s="10"/>
     </row>
     <row r="27" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="14"/>
-      <c r="C27" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="D27" s="9" t="s">
+      <c r="B27" s="15"/>
+      <c r="C27" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="E27" s="9"/>
-      <c r="F27" s="9"/>
+      <c r="D27" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="E27" s="10"/>
+      <c r="F27" s="10"/>
     </row>
     <row r="28" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="14"/>
-      <c r="C28" s="9" t="s">
-        <v>103</v>
-      </c>
-      <c r="D28" s="9" t="s">
+      <c r="B28" s="15"/>
+      <c r="C28" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="E28" s="9"/>
-      <c r="F28" s="9"/>
+      <c r="D28" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="E28" s="10"/>
+      <c r="F28" s="10"/>
     </row>
     <row r="29" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="14"/>
-      <c r="C29" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="D29" s="9" t="s">
+      <c r="B29" s="15"/>
+      <c r="C29" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="E29" s="9"/>
-      <c r="F29" s="9"/>
+      <c r="D29" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="E29" s="10"/>
+      <c r="F29" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1428,9 +1446,6 @@
     <mergeCell ref="B11:B23"/>
     <mergeCell ref="B25:B29"/>
   </mergeCells>
-  <hyperlinks>
-    <hyperlink ref="E3" r:id="rId1" display="arjan.bink@silabs.com"/>
-  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -1452,7 +1467,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.42"/>
@@ -1464,228 +1479,228 @@
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2" s="4" t="s">
+      <c r="B2" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="C2" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F2" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="G2" s="4" t="s">
+      <c r="D2" s="5" t="s">
         <v>20</v>
       </c>
+      <c r="E2" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B3" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="C3" s="7" t="s">
+      <c r="B3" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="C3" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="E3" s="8"/>
-      <c r="F3" s="7" t="s">
+      <c r="D3" s="8" t="s">
         <v>111</v>
       </c>
-      <c r="G3" s="7" t="s">
+      <c r="E3" s="9"/>
+      <c r="F3" s="8" t="s">
         <v>112</v>
       </c>
+      <c r="G3" s="8" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="5"/>
-      <c r="C4" s="7" t="s">
+      <c r="B4" s="6"/>
+      <c r="C4" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="E4" s="9"/>
+      <c r="F4" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="G4" s="8" t="s">
         <v>113</v>
       </c>
-      <c r="D4" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="E4" s="8"/>
-      <c r="F4" s="9" t="s">
-        <v>115</v>
-      </c>
-      <c r="G4" s="7" t="s">
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B5" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="E5" s="9"/>
+      <c r="F5" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="7"/>
+      <c r="C6" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="E6" s="9"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="8" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="E7" s="9"/>
+      <c r="F7" s="8" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B5" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>118</v>
-      </c>
-      <c r="E5" s="8"/>
-      <c r="F5" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="G5" s="7" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="6"/>
-      <c r="C6" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>122</v>
-      </c>
-      <c r="E6" s="8"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="7" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>124</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>125</v>
-      </c>
-      <c r="E7" s="8"/>
-      <c r="F7" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="G7" s="7" t="s">
+      <c r="G7" s="8" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="7"/>
+      <c r="C8" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="D8" s="8" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="6"/>
-      <c r="C8" s="7" t="s">
+      <c r="E8" s="9"/>
+      <c r="F8" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="G8" s="8" t="s">
         <v>127</v>
       </c>
-      <c r="D8" s="7" t="s">
-        <v>125</v>
-      </c>
-      <c r="E8" s="8"/>
-      <c r="F8" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="G8" s="7" t="s">
-        <v>126</v>
-      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="6"/>
-      <c r="C9" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="D9" s="15" t="n">
+      <c r="B9" s="7"/>
+      <c r="C9" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="D9" s="16" t="n">
         <v>1</v>
       </c>
-      <c r="E9" s="16"/>
-      <c r="F9" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="G9" s="7" t="s">
-        <v>126</v>
+      <c r="E9" s="17"/>
+      <c r="F9" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="6"/>
-      <c r="C10" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="D10" s="15" t="n">
+      <c r="B10" s="7"/>
+      <c r="C10" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="D10" s="16" t="n">
         <v>1</v>
       </c>
-      <c r="E10" s="16"/>
-      <c r="F10" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="G10" s="7" t="s">
-        <v>126</v>
+      <c r="E10" s="17"/>
+      <c r="F10" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="C11" s="7" t="s">
+      <c r="B11" s="7" t="s">
         <v>131</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="C11" s="8" t="s">
         <v>132</v>
       </c>
-      <c r="E11" s="8"/>
-      <c r="F11" s="7" t="s">
+      <c r="D11" s="8" t="s">
         <v>133</v>
       </c>
-      <c r="G11" s="7" t="s">
-        <v>112</v>
+      <c r="E11" s="9"/>
+      <c r="F11" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="6"/>
-      <c r="C12" s="7" t="s">
+      <c r="B12" s="7"/>
+      <c r="C12" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="E12" s="9"/>
+      <c r="F12" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="D12" s="7" t="s">
-        <v>135</v>
-      </c>
-      <c r="E12" s="8"/>
-      <c r="F12" s="7" t="s">
-        <v>133</v>
-      </c>
-      <c r="G12" s="7" t="s">
-        <v>126</v>
+      <c r="G12" s="8" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B13" s="6" t="s">
-        <v>136</v>
-      </c>
-      <c r="C13" s="7" t="s">
+      <c r="B13" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="D13" s="7"/>
-      <c r="E13" s="17"/>
-      <c r="F13" s="7" t="s">
-        <v>133</v>
-      </c>
-      <c r="G13" s="7"/>
+      <c r="C13" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="D13" s="8"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="G13" s="8"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="6"/>
-      <c r="C14" s="7" t="s">
-        <v>138</v>
-      </c>
-      <c r="D14" s="7"/>
-      <c r="E14" s="17"/>
-      <c r="F14" s="7" t="s">
-        <v>133</v>
-      </c>
-      <c r="G14" s="7"/>
+      <c r="B14" s="7"/>
+      <c r="C14" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="D14" s="8"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="G14" s="8"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="6"/>
-      <c r="C15" s="7" t="s">
-        <v>139</v>
-      </c>
-      <c r="D15" s="7"/>
-      <c r="E15" s="17"/>
-      <c r="F15" s="7" t="s">
-        <v>133</v>
-      </c>
-      <c r="G15" s="7"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="D15" s="8"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="G15" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -1713,11 +1728,11 @@
   </sheetPr>
   <dimension ref="B2:F3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.42"/>
@@ -1728,35 +1743,35 @@
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2" s="4" t="s">
+      <c r="B2" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="C2" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="D2" s="5" t="s">
         <v>20</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="0" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="E3" s="18"/>
+        <v>143</v>
+      </c>
+      <c r="E3" s="19"/>
       <c r="F3" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
   </sheetData>

</xml_diff>